<commit_message>
Add shortcuts for acrobat pdf reader
</commit_message>
<xml_diff>
--- a/computer/shortcuts/win-mac-dev-util.xlsx
+++ b/computer/shortcuts/win-mac-dev-util.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i348151/workspace/github/knowledge-n-tools/computer/shortcuts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CAEC89-0248-CD42-B5CE-7F0ABDBA80E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE4305E-927E-B048-82B2-D560062F7861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16380" xr2:uid="{BBC1CA9D-A7C2-A04E-A47E-88F2ED23C0E5}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BBC1CA9D-A7C2-A04E-A47E-88F2ED23C0E5}"/>
   </bookViews>
   <sheets>
     <sheet name="OS" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="129">
   <si>
     <t>Intellij Idea</t>
   </si>
@@ -197,9 +197,6 @@
     <t>tmux ls</t>
   </si>
   <si>
-    <t>tmux attach-session -t abc</t>
-  </si>
-  <si>
     <t>Wox open folder</t>
   </si>
   <si>
@@ -377,6 +374,57 @@
   </si>
   <si>
     <t>Open file in another  window</t>
+  </si>
+  <si>
+    <t>Move app to Monitor</t>
+  </si>
+  <si>
+    <t>Win+Shift+Left</t>
+  </si>
+  <si>
+    <t>tmux create window</t>
+  </si>
+  <si>
+    <t>tmux jump windows</t>
+  </si>
+  <si>
+    <t>tmux attach-session -t abc / tmux a #</t>
+  </si>
+  <si>
+    <t>list sessions</t>
+  </si>
+  <si>
+    <t>C+b c</t>
+  </si>
+  <si>
+    <t>C+b n/p   % "</t>
+  </si>
+  <si>
+    <t>C+M+=</t>
+  </si>
+  <si>
+    <t>ShowHide</t>
+  </si>
+  <si>
+    <t>M+x set-file-mode 0666</t>
+  </si>
+  <si>
+    <t>021-6030 8633</t>
+  </si>
+  <si>
+    <t>PDF</t>
+  </si>
+  <si>
+    <t>Ctrl+Y</t>
+  </si>
+  <si>
+    <t>Full screen</t>
+  </si>
+  <si>
+    <t>Ctrl+L</t>
+  </si>
+  <si>
+    <t>Zoom Menu</t>
   </si>
 </sst>
 </file>
@@ -425,15 +473,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thick">
         <color auto="1"/>
       </right>
@@ -443,9 +482,18 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF92D050"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -454,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -468,46 +516,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -515,8 +543,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="distributed" wrapText="1"/>
@@ -837,441 +884,517 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D02C41-EE36-3547-A2D0-C727C78DBCF1}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A14" zoomScale="125" zoomScaleNormal="184" zoomScaleSheetLayoutView="143" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="125" zoomScaleNormal="184" zoomScaleSheetLayoutView="143" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" style="12" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="21.1640625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="0.83203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="0.6640625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="1.1640625" style="12" customWidth="1"/>
-    <col min="7" max="7" width="4.6640625" style="12" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" style="12" customWidth="1"/>
-    <col min="9" max="9" width="20.1640625" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="21.33203125" style="12"/>
+    <col min="1" max="1" width="9" style="8" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="21.1640625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="0.83203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="0.6640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="1.1640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="21.33203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="16"/>
+      <c r="H2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="24"/>
-      <c r="H2" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="16"/>
+      <c r="H3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="16"/>
+      <c r="H4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="16"/>
+      <c r="H7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="24"/>
-      <c r="H3" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="24"/>
-      <c r="H4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="24"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="24"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="24"/>
-      <c r="H7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="12" t="s">
+      <c r="C8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="16"/>
+      <c r="H8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="H8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
+      <c r="C9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="16"/>
+      <c r="H9" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="16"/>
+      <c r="H10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="H9" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="24"/>
-      <c r="H10" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="14" t="s">
+      <c r="C11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="16"/>
+    </row>
+    <row r="12" spans="1:14" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="22"/>
+      <c r="B12" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="24"/>
-    </row>
-    <row r="12" spans="1:14" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14" t="s">
+      <c r="C12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+    </row>
+    <row r="13" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="22"/>
+      <c r="B13" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-    </row>
-    <row r="13" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="26"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="14" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="14"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="10"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="4"/>
       <c r="H14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="8" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="15"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>57</v>
+      <c r="I15" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="15"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="12" t="s">
+      <c r="H16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I17" s="23" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="20" t="s">
+    <row r="18" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="4"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="4"/>
-      <c r="I18" s="8"/>
-    </row>
-    <row r="19" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+      <c r="C19" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="9"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="4"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+    </row>
+    <row r="22" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="4"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="24"/>
-      <c r="G20" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-    </row>
-    <row r="21" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="24"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="12" t="s">
+      <c r="I22" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="I21" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="24"/>
-      <c r="G22" s="4"/>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="24"/>
-      <c r="G23" s="20" t="s">
+    </row>
+    <row r="23" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="4"/>
+      <c r="I23" s="20"/>
+    </row>
+    <row r="24" spans="1:12" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-    </row>
-    <row r="24" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="E24" s="24"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="12" t="s">
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="I25" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="E25" s="24"/>
-      <c r="G25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="E26" s="24"/>
-      <c r="H26" s="12" t="s">
+    <row r="26" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="16"/>
+      <c r="H27" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="E27" s="24"/>
-      <c r="H27" s="12" t="s">
+    <row r="28" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="16"/>
+      <c r="H28" s="8" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="E28" s="24"/>
-      <c r="H28" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="E29" s="24"/>
-    </row>
-    <row r="30" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="E30" s="24"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="E31" s="24"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="E32" s="24"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E33" s="24"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E34" s="24"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E35" s="24"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E36" s="24"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E37" s="24"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E38" s="24"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E39" s="24"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E40" s="24"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="24"/>
+      <c r="I28" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="16"/>
+      <c r="H29" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="16"/>
+      <c r="H30" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="16"/>
+      <c r="H31" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="16"/>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="9"/>
+      <c r="F33" s="16"/>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="9"/>
+      <c r="F34" s="16"/>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E35" s="9"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E36" s="9"/>
+      <c r="F36" s="16"/>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E37" s="9"/>
+      <c r="F37" s="16"/>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E38" s="9"/>
+      <c r="F38" s="16"/>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E39" s="9"/>
+      <c r="F39" s="16"/>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E40" s="9"/>
+      <c r="F40" s="16"/>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E41" s="9"/>
+      <c r="F41" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="I21:I22"/>
+  <mergeCells count="14">
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="I22:I23"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="B14:B15"/>
@@ -1280,7 +1403,9 @@
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="G12:N12"/>
-    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A21:C21"/>
   </mergeCells>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.35" header="0.1" footer="0.1"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1289,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58534F79-26B5-B64A-8061-31B273BB9A7B}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A29" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1304,27 +1429,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>38</v>
@@ -1333,7 +1460,7 @@
     <row r="4" spans="1:3" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>39</v>
@@ -1342,37 +1469,37 @@
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="8" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="9"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="25"/>
     </row>
     <row r="9" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>32</v>
@@ -1380,10 +1507,10 @@
     </row>
     <row r="10" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.25">
@@ -1391,20 +1518,20 @@
         <v>44</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="27"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
     </row>
     <row r="14" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
@@ -1413,10 +1540,10 @@
     </row>
     <row r="15" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>47</v>
@@ -1424,38 +1551,38 @@
     </row>
     <row r="16" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C18" s="9" t="s">
+      <c r="B18" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="25" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="9"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="25"/>
     </row>
     <row r="20" spans="1:3" ht="20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>45</v>
@@ -1466,40 +1593,51 @@
     </row>
     <row r="21" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="3" t="s">
+    </row>
+    <row r="22" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-    </row>
+    <row r="25" spans="1:3" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>